<commit_message>
descripción de puesto, organigrama y, listado de docs
Agregue la descripción de puestos, modifique y mejore el organigrama, y modifique el listado de docs
</commit_message>
<xml_diff>
--- a/listado docs ctrl Proyectos.xlsx
+++ b/listado docs ctrl Proyectos.xlsx
@@ -1,12 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
+  <workbookPr defaultThemeVersion="124226"/>
+  <bookViews>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="550"/>
+  </bookViews>
   <sheets>
-    <sheet state="visible" name="Hoja 1" sheetId="1" r:id="rId3"/>
+    <sheet name="Hoja 1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <definedNames/>
-  <calcPr/>
+  <calcPr calcId="125725"/>
 </workbook>
 </file>
 
@@ -118,21 +121,35 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="3">
     <font>
-      <sz val="10.0"/>
+      <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
     </font>
-    <font/>
+    <font>
+      <sz val="11"/>
+      <name val="Cambria"/>
+      <family val="1"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <strike/>
+      <sz val="11"/>
+      <name val="Cambria"/>
+      <family val="1"/>
+      <charset val="1"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
-      <patternFill patternType="lightGray"/>
+      <patternFill patternType="gray125"/>
     </fill>
   </fills>
   <borders count="1">
@@ -141,41 +158,323 @@
       <right/>
       <top/>
       <bottom/>
+      <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment/>
-    </xf>
+  <cellXfs count="3">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle xfId="0" name="Normal" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
 </styleSheet>
 </file>
 
-<file path=xl/drawings/worksheetdrawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram"/>
+<file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+  <a:themeElements>
+    <a:clrScheme name="Office">
+      <a:dk1>
+        <a:sysClr val="windowText" lastClr="000000"/>
+      </a:dk1>
+      <a:lt1>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
+      </a:lt1>
+      <a:dk2>
+        <a:srgbClr val="1F497D"/>
+      </a:dk2>
+      <a:lt2>
+        <a:srgbClr val="EEECE1"/>
+      </a:lt2>
+      <a:accent1>
+        <a:srgbClr val="4F81BD"/>
+      </a:accent1>
+      <a:accent2>
+        <a:srgbClr val="C0504D"/>
+      </a:accent2>
+      <a:accent3>
+        <a:srgbClr val="9BBB59"/>
+      </a:accent3>
+      <a:accent4>
+        <a:srgbClr val="8064A2"/>
+      </a:accent4>
+      <a:accent5>
+        <a:srgbClr val="4BACC6"/>
+      </a:accent5>
+      <a:accent6>
+        <a:srgbClr val="F79646"/>
+      </a:accent6>
+      <a:hlink>
+        <a:srgbClr val="0000FF"/>
+      </a:hlink>
+      <a:folHlink>
+        <a:srgbClr val="800080"/>
+      </a:folHlink>
+    </a:clrScheme>
+    <a:fontScheme name="Office">
+      <a:majorFont>
+        <a:latin typeface="Cambria"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Times New Roman"/>
+        <a:font script="Hebr" typeface="Times New Roman"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="MoolBoran"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Times New Roman"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+      </a:majorFont>
+      <a:minorFont>
+        <a:latin typeface="Calibri"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Arial"/>
+        <a:font script="Hebr" typeface="Arial"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="DaunPenh"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Arial"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+      </a:minorFont>
+    </a:fontScheme>
+    <a:fmtScheme name="Office">
+      <a:fillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="50000"/>
+                <a:satMod val="300000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="35000">
+              <a:schemeClr val="phClr">
+                <a:tint val="37000"/>
+                <a:satMod val="300000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:tint val="15000"/>
+                <a:satMod val="350000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="16200000" scaled="1"/>
+        </a:gradFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:shade val="51000"/>
+                <a:satMod val="130000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="80000">
+              <a:schemeClr val="phClr">
+                <a:shade val="93000"/>
+                <a:satMod val="130000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:shade val="94000"/>
+                <a:satMod val="135000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="16200000" scaled="0"/>
+        </a:gradFill>
+      </a:fillStyleLst>
+      <a:lnStyleLst>
+        <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr">
+              <a:shade val="95000"/>
+              <a:satMod val="105000"/>
+            </a:schemeClr>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+        </a:ln>
+        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+        </a:ln>
+        <a:ln w="38100" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+        </a:ln>
+      </a:lnStyleLst>
+      <a:effectStyleLst>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw blurRad="40000" dist="20000" dir="5400000" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="38000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="35000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="35000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+          <a:scene3d>
+            <a:camera prst="orthographicFront">
+              <a:rot lat="0" lon="0" rev="0"/>
+            </a:camera>
+            <a:lightRig rig="threePt" dir="t">
+              <a:rot lat="0" lon="0" rev="1200000"/>
+            </a:lightRig>
+          </a:scene3d>
+          <a:sp3d>
+            <a:bevelT w="63500" h="25400"/>
+          </a:sp3d>
+        </a:effectStyle>
+      </a:effectStyleLst>
+      <a:bgFillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="40000"/>
+                <a:satMod val="350000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="40000">
+              <a:schemeClr val="phClr">
+                <a:tint val="45000"/>
+                <a:shade val="99000"/>
+                <a:satMod val="350000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:shade val="20000"/>
+                <a:satMod val="255000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:path path="circle">
+            <a:fillToRect l="50000" t="-80000" r="50000" b="180000"/>
+          </a:path>
+        </a:gradFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="80000"/>
+                <a:satMod val="300000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:shade val="30000"/>
+                <a:satMod val="200000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:path path="circle">
+            <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
+          </a:path>
+        </a:gradFill>
+      </a:bgFillStyleLst>
+    </a:fmtScheme>
+  </a:themeElements>
+  <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
+</a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:F33"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E12" sqref="E12"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.75"/>
+  <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
-    <col customWidth="1" min="1" max="1" width="26.43"/>
+    <col min="1" max="1" width="26.42578125"/>
+    <col min="2" max="1025" width="14.42578125"/>
   </cols>
   <sheetData>
-    <row r="1">
+    <row r="1" spans="1:6" ht="14.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -183,7 +482,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2">
+    <row r="2" spans="1:6" ht="14.25">
       <c r="A2" s="1" t="s">
         <v>2</v>
       </c>
@@ -194,14 +493,14 @@
         <v>4</v>
       </c>
       <c r="E2" s="1">
-        <v>6.0</v>
-      </c>
-      <c r="F2" t="str">
-        <f t="shared" ref="F2:F6" si="1">COUNTIF(B1:B33,D2)</f>
-        <v>6</v>
-      </c>
-    </row>
-    <row r="3">
+        <v>6</v>
+      </c>
+      <c r="F2">
+        <f>COUNTIF(B1:B33,D2)</f>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" ht="14.25">
       <c r="A3" s="1" t="s">
         <v>5</v>
       </c>
@@ -212,14 +511,14 @@
         <v>7</v>
       </c>
       <c r="E3" s="1">
-        <v>6.0</v>
-      </c>
-      <c r="F3" t="str">
-        <f t="shared" si="1"/>
-        <v>6</v>
-      </c>
-    </row>
-    <row r="4">
+        <v>6</v>
+      </c>
+      <c r="F3">
+        <f>COUNTIF(B2:B34,D3)</f>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" ht="14.25">
       <c r="A4" s="1" t="s">
         <v>8</v>
       </c>
@@ -230,50 +529,50 @@
         <v>6</v>
       </c>
       <c r="E4" s="1">
-        <v>6.0</v>
-      </c>
-      <c r="F4" t="str">
-        <f t="shared" si="1"/>
+        <v>6</v>
+      </c>
+      <c r="F4">
+        <f>COUNTIF(B3:B35,D4)</f>
         <v>5</v>
       </c>
     </row>
-    <row r="5">
-      <c r="A5" s="1" t="s">
+    <row r="5" spans="1:6" ht="14.25">
+      <c r="A5" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="B5" s="1" t="s">
+      <c r="B5" s="2" t="s">
         <v>4</v>
       </c>
       <c r="D5" s="1" t="s">
         <v>1</v>
       </c>
       <c r="E5" s="1">
-        <v>6.0</v>
-      </c>
-      <c r="F5" t="str">
-        <f t="shared" si="1"/>
+        <v>6</v>
+      </c>
+      <c r="F5">
+        <f>COUNTIF(B4:B36,D5)</f>
         <v>5</v>
       </c>
     </row>
-    <row r="6">
-      <c r="A6" s="1" t="s">
+    <row r="6" spans="1:6" ht="14.25">
+      <c r="A6" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="B6" s="1" t="s">
-        <v>7</v>
+      <c r="B6" s="2" t="s">
+        <v>4</v>
       </c>
       <c r="D6" s="1" t="s">
         <v>3</v>
       </c>
       <c r="E6" s="1">
-        <v>5.0</v>
-      </c>
-      <c r="F6" t="str">
-        <f t="shared" si="1"/>
         <v>5</v>
       </c>
-    </row>
-    <row r="8">
+      <c r="F6">
+        <f>COUNTIF(B5:B37,D6)</f>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" ht="14.25">
       <c r="A8" s="1" t="s">
         <v>11</v>
       </c>
@@ -281,7 +580,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="9">
+    <row r="9" spans="1:6" ht="14.25">
       <c r="A9" s="1" t="s">
         <v>12</v>
       </c>
@@ -289,7 +588,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="10">
+    <row r="10" spans="1:6" ht="14.25">
       <c r="A10" s="1" t="s">
         <v>13</v>
       </c>
@@ -297,7 +596,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="11">
+    <row r="11" spans="1:6" ht="14.25">
       <c r="A11" s="1" t="s">
         <v>14</v>
       </c>
@@ -305,7 +604,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="12">
+    <row r="12" spans="1:6" ht="14.25">
       <c r="A12" s="1" t="s">
         <v>15</v>
       </c>
@@ -313,7 +612,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13">
+    <row r="13" spans="1:6" ht="14.25">
       <c r="A13" s="1" t="s">
         <v>16</v>
       </c>
@@ -321,7 +620,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="15">
+    <row r="15" spans="1:6" ht="14.25">
       <c r="A15" s="1" t="s">
         <v>17</v>
       </c>
@@ -329,7 +628,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="16">
+    <row r="16" spans="1:6" ht="14.25">
       <c r="A16" s="1" t="s">
         <v>18</v>
       </c>
@@ -337,7 +636,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17">
+    <row r="17" spans="1:2" ht="14.25">
       <c r="A17" s="1" t="s">
         <v>19</v>
       </c>
@@ -345,7 +644,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="18">
+    <row r="18" spans="1:2" ht="14.25">
       <c r="A18" s="1" t="s">
         <v>20</v>
       </c>
@@ -353,7 +652,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="19">
+    <row r="19" spans="1:2" ht="14.25">
       <c r="A19" s="1" t="s">
         <v>21</v>
       </c>
@@ -361,7 +660,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="21">
+    <row r="21" spans="1:2" ht="14.25">
       <c r="A21" s="1" t="s">
         <v>22</v>
       </c>
@@ -369,7 +668,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="22">
+    <row r="22" spans="1:2" ht="14.25">
       <c r="A22" s="1" t="s">
         <v>23</v>
       </c>
@@ -377,7 +676,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="23">
+    <row r="23" spans="1:2" ht="14.25">
       <c r="A23" s="1" t="s">
         <v>24</v>
       </c>
@@ -385,7 +684,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="24">
+    <row r="24" spans="1:2" ht="14.25">
       <c r="A24" s="1" t="s">
         <v>25</v>
       </c>
@@ -393,7 +692,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="25">
+    <row r="25" spans="1:2" ht="14.25">
       <c r="A25" s="1" t="s">
         <v>26</v>
       </c>
@@ -401,7 +700,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="26">
+    <row r="26" spans="1:2" ht="14.25">
       <c r="A26" s="1" t="s">
         <v>27</v>
       </c>
@@ -409,7 +708,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="28">
+    <row r="28" spans="1:2" ht="14.25">
       <c r="A28" s="1" t="s">
         <v>28</v>
       </c>
@@ -417,7 +716,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="29">
+    <row r="29" spans="1:2" ht="14.25">
       <c r="A29" s="1" t="s">
         <v>29</v>
       </c>
@@ -425,7 +724,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="30">
+    <row r="30" spans="1:2" ht="14.25">
       <c r="A30" s="1" t="s">
         <v>30</v>
       </c>
@@ -433,7 +732,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="31">
+    <row r="31" spans="1:2" ht="14.25">
       <c r="A31" s="1" t="s">
         <v>31</v>
       </c>
@@ -441,7 +740,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="32">
+    <row r="32" spans="1:2" ht="14.25">
       <c r="A32" s="1" t="s">
         <v>32</v>
       </c>
@@ -449,15 +748,16 @@
         <v>7</v>
       </c>
     </row>
-    <row r="33">
+    <row r="33" spans="1:2" ht="14.25">
       <c r="A33" s="1" t="s">
         <v>33</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>4</v>
+        <v>7</v>
       </c>
     </row>
   </sheetData>
-  <drawing r:id="rId1"/>
+  <pageMargins left="0.74791666666666701" right="0.74791666666666701" top="0.98402777777777795" bottom="0.98402777777777795" header="0.51180555555555496" footer="0.51180555555555496"/>
+  <pageSetup firstPageNumber="0" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Actualizacion de Lista de Documentos
</commit_message>
<xml_diff>
--- a/listado docs ctrl Proyectos.xlsx
+++ b/listado docs ctrl Proyectos.xlsx
@@ -1,15 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Nacho Martinez\Desktop\Control-de-Proyectos\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="550"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja 1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="125725"/>
+  <calcPr calcId="152511"/>
 </workbook>
 </file>
 
@@ -49,9 +54,6 @@
     <t>descripciones de puesto</t>
   </si>
   <si>
-    <t>lista de errores</t>
-  </si>
-  <si>
     <t>matriz de responsabilidades</t>
   </si>
   <si>
@@ -116,13 +118,16 @@
   </si>
   <si>
     <t>respuesta ante el riesgo</t>
+  </si>
+  <si>
+    <t>lista de Roles</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="3">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -144,12 +149,18 @@
       <charset val="1"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -164,21 +175,30 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema de Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -220,7 +240,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -252,9 +272,10 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -286,6 +307,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -461,32 +483,32 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F33"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E12" sqref="E12"/>
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="26.42578125"/>
     <col min="2" max="1025" width="14.42578125"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="14.25">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:6" ht="14.25" x14ac:dyDescent="0.2">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="14.25">
-      <c r="A2" s="1" t="s">
+    <row r="2" spans="1:6" ht="14.25" x14ac:dyDescent="0.2">
+      <c r="A2" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="B2" s="2" t="s">
         <v>3</v>
       </c>
       <c r="D2" s="1" t="s">
@@ -500,11 +522,11 @@
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="14.25">
-      <c r="A3" s="1" t="s">
+    <row r="3" spans="1:6" ht="14.25" x14ac:dyDescent="0.2">
+      <c r="A3" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="B3" s="1" t="s">
+      <c r="B3" s="2" t="s">
         <v>6</v>
       </c>
       <c r="D3" s="1" t="s">
@@ -518,7 +540,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="1:6" ht="14.25">
+    <row r="4" spans="1:6" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>8</v>
       </c>
@@ -536,11 +558,11 @@
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="1:6" ht="14.25">
-      <c r="A5" s="2" t="s">
+    <row r="5" spans="1:6" ht="14.25" x14ac:dyDescent="0.2">
+      <c r="A5" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="B5" s="2" t="s">
+      <c r="B5" s="3" t="s">
         <v>4</v>
       </c>
       <c r="D5" s="1" t="s">
@@ -554,11 +576,11 @@
         <v>5</v>
       </c>
     </row>
-    <row r="6" spans="1:6" ht="14.25">
-      <c r="A6" s="2" t="s">
+    <row r="6" spans="1:6" ht="14.25" x14ac:dyDescent="0.2">
+      <c r="A6" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="B6" s="2" t="s">
+      <c r="B6" s="3" t="s">
         <v>4</v>
       </c>
       <c r="D6" s="1" t="s">
@@ -572,185 +594,185 @@
         <v>5</v>
       </c>
     </row>
-    <row r="8" spans="1:6" ht="14.25">
-      <c r="A8" s="1" t="s">
+    <row r="8" spans="1:6" ht="14.25" x14ac:dyDescent="0.2">
+      <c r="A8" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" ht="14.25" x14ac:dyDescent="0.2">
+      <c r="A9" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="B8" s="1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" ht="14.25">
-      <c r="A9" s="1" t="s">
+      <c r="B9" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" ht="14.25" x14ac:dyDescent="0.2">
+      <c r="A10" s="1" t="s">
         <v>12</v>
-      </c>
-      <c r="B9" s="1" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" ht="14.25">
-      <c r="A10" s="1" t="s">
-        <v>13</v>
       </c>
       <c r="B10" s="1" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="11" spans="1:6" ht="14.25">
-      <c r="A11" s="1" t="s">
+    <row r="11" spans="1:6" ht="14.25" x14ac:dyDescent="0.2">
+      <c r="A11" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" ht="14.25" x14ac:dyDescent="0.2">
+      <c r="A12" s="1" t="s">
         <v>14</v>
-      </c>
-      <c r="B11" s="1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" ht="14.25">
-      <c r="A12" s="1" t="s">
-        <v>15</v>
       </c>
       <c r="B12" s="1" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:6" ht="14.25">
-      <c r="A13" s="1" t="s">
+    <row r="13" spans="1:6" ht="14.25" x14ac:dyDescent="0.2">
+      <c r="A13" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" ht="14.25" x14ac:dyDescent="0.2">
+      <c r="A15" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="B13" s="1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6" ht="14.25">
-      <c r="A15" s="1" t="s">
+      <c r="B15" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" ht="14.25" x14ac:dyDescent="0.2">
+      <c r="A16" s="1" t="s">
         <v>17</v>
-      </c>
-      <c r="B15" s="1" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6" ht="14.25">
-      <c r="A16" s="1" t="s">
-        <v>18</v>
       </c>
       <c r="B16" s="1" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:2" ht="14.25">
+    <row r="17" spans="1:2" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A17" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B17" s="1" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="18" spans="1:2" ht="14.25">
+    <row r="18" spans="1:2" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A18" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B18" s="1" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="19" spans="1:2" ht="14.25">
+    <row r="19" spans="1:2" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A19" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B19" s="1" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="21" spans="1:2" ht="14.25">
+    <row r="21" spans="1:2" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A21" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" ht="14.25" x14ac:dyDescent="0.2">
+      <c r="A22" s="1" t="s">
         <v>22</v>
-      </c>
-      <c r="B21" s="1" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="22" spans="1:2" ht="14.25">
-      <c r="A22" s="1" t="s">
-        <v>23</v>
       </c>
       <c r="B22" s="1" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="23" spans="1:2" ht="14.25">
-      <c r="A23" s="1" t="s">
+    <row r="23" spans="1:2" ht="14.25" x14ac:dyDescent="0.2">
+      <c r="A23" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="B23" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" ht="14.25" x14ac:dyDescent="0.2">
+      <c r="A24" s="1" t="s">
         <v>24</v>
-      </c>
-      <c r="B23" s="1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="24" spans="1:2" ht="14.25">
-      <c r="A24" s="1" t="s">
-        <v>25</v>
       </c>
       <c r="B24" s="1" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="25" spans="1:2" ht="14.25">
-      <c r="A25" s="1" t="s">
+    <row r="25" spans="1:2" ht="14.25" x14ac:dyDescent="0.2">
+      <c r="A25" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="B25" s="2" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" ht="14.25" x14ac:dyDescent="0.2">
+      <c r="A26" s="1" t="s">
         <v>26</v>
-      </c>
-      <c r="B25" s="1" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="26" spans="1:2" ht="14.25">
-      <c r="A26" s="1" t="s">
-        <v>27</v>
       </c>
       <c r="B26" s="1" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="28" spans="1:2" ht="14.25">
+    <row r="28" spans="1:2" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A28" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="B28" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" ht="14.25" x14ac:dyDescent="0.2">
+      <c r="A29" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="B28" s="1" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="29" spans="1:2" ht="14.25">
-      <c r="A29" s="1" t="s">
+      <c r="B29" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" ht="14.25" x14ac:dyDescent="0.2">
+      <c r="A30" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="B29" s="1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="30" spans="1:2" ht="14.25">
-      <c r="A30" s="1" t="s">
+      <c r="B30" s="2" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" ht="14.25" x14ac:dyDescent="0.2">
+      <c r="A31" s="1" t="s">
         <v>30</v>
-      </c>
-      <c r="B30" s="1" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="31" spans="1:2" ht="14.25">
-      <c r="A31" s="1" t="s">
-        <v>31</v>
       </c>
       <c r="B31" s="1" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="32" spans="1:2" ht="14.25">
-      <c r="A32" s="1" t="s">
+    <row r="32" spans="1:2" ht="14.25" x14ac:dyDescent="0.2">
+      <c r="A32" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="B32" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" ht="14.25" x14ac:dyDescent="0.2">
+      <c r="A33" s="1" t="s">
         <v>32</v>
-      </c>
-      <c r="B32" s="1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="33" spans="1:2" ht="14.25">
-      <c r="A33" s="1" t="s">
-        <v>33</v>
       </c>
       <c r="B33" s="1" t="s">
         <v>7</v>

</xml_diff>

<commit_message>
correccion agenda/diagrama de gantt
</commit_message>
<xml_diff>
--- a/listado docs ctrl Proyectos.xlsx
+++ b/listado docs ctrl Proyectos.xlsx
@@ -487,7 +487,7 @@
   <dimension ref="A1:F33"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B19" sqref="B19"/>
+      <selection activeCell="G10" sqref="G10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -691,10 +691,10 @@
       </c>
     </row>
     <row r="22" spans="1:2" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A22" s="1" t="s">
+      <c r="A22" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="B22" s="1" t="s">
+      <c r="B22" s="2" t="s">
         <v>7</v>
       </c>
     </row>
@@ -707,10 +707,10 @@
       </c>
     </row>
     <row r="24" spans="1:2" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A24" s="1" t="s">
+      <c r="A24" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="B24" s="1" t="s">
+      <c r="B24" s="2" t="s">
         <v>4</v>
       </c>
     </row>

</xml_diff>